<commit_message>
added lin reg equations
</commit_message>
<xml_diff>
--- a/Diastole BP Updated.xlsx
+++ b/Diastole BP Updated.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -750,6 +750,22 @@
         <v>102.290555</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>73.93605490000002</v>
+      </c>
+      <c r="B40" t="n">
+        <v>115.284784</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>79.97993409999999</v>
+      </c>
+      <c r="B41" t="n">
+        <v>111.490211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>